<commit_message>
all adds up analysis
</commit_message>
<xml_diff>
--- a/input/Financial Statement AAPL/Sales By Segment.xlsx
+++ b/input/Financial Statement AAPL/Sales By Segment.xlsx
@@ -604,7 +604,7 @@
         <v>24846</v>
       </c>
       <c r="F2" t="n">
-        <v>116473</v>
+        <v>28846</v>
       </c>
       <c r="G2" t="n">
         <v>141319</v>
@@ -619,7 +619,7 @@
         <v>29906</v>
       </c>
       <c r="K2" t="n">
-        <v>136793</v>
+        <v>37185</v>
       </c>
       <c r="L2" t="n">
         <v>166699</v>
@@ -634,7 +634,7 @@
         <v>25986</v>
       </c>
       <c r="P2" t="n">
-        <v>116395</v>
+        <v>33362</v>
       </c>
       <c r="Q2" t="n">
         <v>142381</v>
@@ -649,7 +649,7 @@
         <v>26418</v>
       </c>
       <c r="U2" t="n">
-        <v>111363</v>
+        <v>26444</v>
       </c>
       <c r="V2" t="n">
         <v>137781</v>
@@ -664,7 +664,7 @@
         <v>39570</v>
       </c>
       <c r="Z2" t="n">
-        <v>152403</v>
+        <v>38868</v>
       </c>
       <c r="AA2" t="n">
         <v>191973</v>
@@ -698,7 +698,7 @@
         <v>5592</v>
       </c>
       <c r="F3" t="n">
-        <v>20258</v>
+        <v>7170</v>
       </c>
       <c r="G3" t="n">
         <v>25850</v>
@@ -713,7 +713,7 @@
         <v>5330</v>
       </c>
       <c r="K3" t="n">
-        <v>20154</v>
+        <v>7411</v>
       </c>
       <c r="L3" t="n">
         <v>25484</v>
@@ -728,7 +728,7 @@
         <v>5820</v>
       </c>
       <c r="P3" t="n">
-        <v>19920</v>
+        <v>6991</v>
       </c>
       <c r="Q3" t="n">
         <v>25740</v>
@@ -743,7 +743,7 @@
         <v>7079</v>
       </c>
       <c r="U3" t="n">
-        <v>21543</v>
+        <v>9032</v>
       </c>
       <c r="V3" t="n">
         <v>28622</v>
@@ -758,7 +758,7 @@
         <v>8235</v>
       </c>
       <c r="Z3" t="n">
-        <v>26955</v>
+        <v>9178</v>
       </c>
       <c r="AA3" t="n">
         <v>35190</v>
@@ -792,7 +792,7 @@
         <v>4969</v>
       </c>
       <c r="F4" t="n">
-        <v>14253</v>
+        <v>4831</v>
       </c>
       <c r="G4" t="n">
         <v>19222</v>
@@ -807,7 +807,7 @@
         <v>4741</v>
       </c>
       <c r="K4" t="n">
-        <v>14064</v>
+        <v>4089</v>
       </c>
       <c r="L4" t="n">
         <v>18805</v>
@@ -822,7 +822,7 @@
         <v>5023</v>
       </c>
       <c r="P4" t="n">
-        <v>16257</v>
+        <v>4656</v>
       </c>
       <c r="Q4" t="n">
         <v>21280</v>
@@ -837,7 +837,7 @@
         <v>6582</v>
       </c>
       <c r="U4" t="n">
-        <v>17142</v>
+        <v>6797</v>
       </c>
       <c r="V4" t="n">
         <v>23724</v>
@@ -852,7 +852,7 @@
         <v>7368</v>
       </c>
       <c r="Z4" t="n">
-        <v>24494</v>
+        <v>8252</v>
       </c>
       <c r="AA4" t="n">
         <v>31862</v>
@@ -894,7 +894,7 @@
         <v>5525</v>
       </c>
       <c r="P5" t="n">
-        <v>18957</v>
+        <v>6520</v>
       </c>
       <c r="Q5" t="n">
         <v>24482</v>
@@ -909,7 +909,7 @@
         <v>6450</v>
       </c>
       <c r="U5" t="n">
-        <v>24170</v>
+        <v>7876</v>
       </c>
       <c r="V5" t="n">
         <v>30620</v>
@@ -924,7 +924,7 @@
         <v>8775</v>
       </c>
       <c r="Z5" t="n">
-        <v>29592</v>
+        <v>8785</v>
       </c>
       <c r="AA5" t="n">
         <v>38367</v>
@@ -958,7 +958,7 @@
         <v>7266</v>
       </c>
       <c r="F6" t="n">
-        <v>22714</v>
+        <v>8501</v>
       </c>
       <c r="G6" t="n">
         <v>29980</v>
@@ -973,7 +973,7 @@
         <v>9548</v>
       </c>
       <c r="K6" t="n">
-        <v>27642</v>
+        <v>9981</v>
       </c>
       <c r="L6" t="n">
         <v>37190</v>
@@ -988,7 +988,7 @@
         <v>11455</v>
       </c>
       <c r="P6" t="n">
-        <v>34836</v>
+        <v>12511</v>
       </c>
       <c r="Q6" t="n">
         <v>46291</v>
@@ -1003,7 +1003,7 @@
         <v>13156</v>
       </c>
       <c r="U6" t="n">
-        <v>40612</v>
+        <v>14549</v>
       </c>
       <c r="V6" t="n">
         <v>53768</v>
@@ -1018,7 +1018,7 @@
         <v>17486</v>
       </c>
       <c r="Z6" t="n">
-        <v>50939</v>
+        <v>18277</v>
       </c>
       <c r="AA6" t="n">
         <v>68425</v>
@@ -1052,7 +1052,7 @@
         <v>45408</v>
       </c>
       <c r="F7" t="n">
-        <v>183826</v>
+        <v>52579</v>
       </c>
       <c r="G7" t="n">
         <v>229234</v>
@@ -1067,7 +1067,7 @@
         <v>53265</v>
       </c>
       <c r="K7" t="n">
-        <v>212330</v>
+        <v>62900</v>
       </c>
       <c r="L7" t="n">
         <v>265595</v>
@@ -1082,7 +1082,7 @@
         <v>53809</v>
       </c>
       <c r="P7" t="n">
-        <v>206365</v>
+        <v>64040</v>
       </c>
       <c r="Q7" t="n">
         <v>260174</v>
@@ -1097,7 +1097,7 @@
         <v>59685</v>
       </c>
       <c r="U7" t="n">
-        <v>214830</v>
+        <v>64698</v>
       </c>
       <c r="V7" t="n">
         <v>274515</v>
@@ -1112,7 +1112,7 @@
         <v>81434</v>
       </c>
       <c r="Z7" t="n">
-        <v>284383</v>
+        <v>83360</v>
       </c>
       <c r="AA7" t="n">
         <v>365817</v>
@@ -1146,7 +1146,7 @@
         <v>2735</v>
       </c>
       <c r="F8" t="n">
-        <v>10128</v>
+        <v>3231</v>
       </c>
       <c r="G8" t="n">
         <v>12863</v>
@@ -1161,7 +1161,7 @@
         <v>3740</v>
       </c>
       <c r="K8" t="n">
-        <v>13677</v>
+        <v>4234</v>
       </c>
       <c r="L8" t="n">
         <v>17417</v>

</xml_diff>